<commit_message>
Agregué contenido en README
</commit_message>
<xml_diff>
--- a/Codes/Prueba.xlsx
+++ b/Codes/Prueba.xlsx
@@ -427,11 +427,15 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>2</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Rango</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
       </c>
     </row>
     <row r="2">

</xml_diff>